<commit_message>
pc_dtv home hacia cloud_work 19/07/24
</commit_message>
<xml_diff>
--- a/VLC_FILES/vlc_parsed_xls.xlsx
+++ b/VLC_FILES/vlc_parsed_xls.xlsx
@@ -1,41 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cnigro\PycharmProjects\pythonProject_01\VLC_FILES\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A1E45D-16FF-4E25-ABBC-46F38024CE05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-120" windowWidth="12312" windowHeight="7356"/>
   </bookViews>
   <sheets>
     <sheet name="vlc_parsed" sheetId="3" r:id="rId1"/>
     <sheet name="vlc_parsed_2" sheetId="1" r:id="rId2"/>
-    <sheet name="vlc_parsed_copia" sheetId="2" r:id="rId3"/>
+    <sheet name="vlc_bk" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="166">
   <si>
     <t>fuente</t>
   </si>
@@ -160,9 +141,6 @@
     <t>ENC2_CHANNEL10_NO FUNCA_200821</t>
   </si>
   <si>
-    <t>srt</t>
-  </si>
-  <si>
     <t>protocolo</t>
   </si>
   <si>
@@ -172,25 +150,376 @@
     <t>puerto</t>
   </si>
   <si>
-    <t>10.10.10.10</t>
-  </si>
-  <si>
-    <t>200.110.220.147</t>
-  </si>
-  <si>
-    <t>200.110.220.148</t>
-  </si>
-  <si>
-    <t>10.10.10.11</t>
-  </si>
-  <si>
     <t>srt://200.110.220.147:12222</t>
+  </si>
+  <si>
+    <t>18_CBC_ECUAVISA P</t>
+  </si>
+  <si>
+    <t>24_LaRed-Chile-P_ABC</t>
+  </si>
+  <si>
+    <t>23_Escuela Plus HD P-CBC_ABC</t>
+  </si>
+  <si>
+    <t>26_TNU_ABC</t>
+  </si>
+  <si>
+    <t>31_canal10uru_ABC_P</t>
+  </si>
+  <si>
+    <t>10_CBC_ABC_POC-OCC</t>
+  </si>
+  <si>
+    <t>57_DnewsChile_ABC</t>
+  </si>
+  <si>
+    <t>UDP</t>
+  </si>
+  <si>
+    <t>10.7.250.101</t>
+  </si>
+  <si>
+    <t>238.77.21.7</t>
+  </si>
+  <si>
+    <t>238.77.21.9</t>
+  </si>
+  <si>
+    <t>238.77.21.1</t>
+  </si>
+  <si>
+    <t>238.77.21.11</t>
+  </si>
+  <si>
+    <t>192.168.10.10</t>
+  </si>
+  <si>
+    <t>238.77.21.6</t>
+  </si>
+  <si>
+    <t>238.77.21.57</t>
+  </si>
+  <si>
+    <t>238.1.4.1</t>
+  </si>
+  <si>
+    <t>udp</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>prueba redundancia</t>
+  </si>
+  <si>
+    <t>10.7.250.105</t>
+  </si>
+  <si>
+    <t>238.77.25.6</t>
+  </si>
+  <si>
+    <t>red2</t>
+  </si>
+  <si>
+    <t>238.77.25.1</t>
+  </si>
+  <si>
+    <t>238.77.21.8</t>
+  </si>
+  <si>
+    <t>ecu</t>
+  </si>
+  <si>
+    <t>10.77.6.13</t>
+  </si>
+  <si>
+    <t>239.195.6.13</t>
+  </si>
+  <si>
+    <t>sumavision01</t>
+  </si>
+  <si>
+    <t>sumavision02</t>
+  </si>
+  <si>
+    <t>239.195.6.14</t>
+  </si>
+  <si>
+    <t>239.195.6.15</t>
+  </si>
+  <si>
+    <t>sumavision0_interna</t>
+  </si>
+  <si>
+    <t>239.195.6.16</t>
+  </si>
+  <si>
+    <t>sumavision03</t>
+  </si>
+  <si>
+    <t>sumavision04</t>
+  </si>
+  <si>
+    <t>sumav_enc2_01</t>
+  </si>
+  <si>
+    <t>10.77.10.13</t>
+  </si>
+  <si>
+    <t>239.195.10.1</t>
+  </si>
+  <si>
+    <t>sumav_enc2_02</t>
+  </si>
+  <si>
+    <t>239.195.10.2</t>
+  </si>
+  <si>
+    <t>suma_enc01_out</t>
+  </si>
+  <si>
+    <t>suma_enc02_out</t>
+  </si>
+  <si>
+    <t>suma_dec01_out</t>
+  </si>
+  <si>
+    <t>10.77.6.113</t>
+  </si>
+  <si>
+    <t>239.195.6.113</t>
+  </si>
+  <si>
+    <t>suma_dec02_out</t>
+  </si>
+  <si>
+    <t>239.195.6.114</t>
+  </si>
+  <si>
+    <t>sumav_enc2_01_bk</t>
+  </si>
+  <si>
+    <t>sumav_enc2_02_bk</t>
+  </si>
+  <si>
+    <t>TATA-SERVER-01</t>
+  </si>
+  <si>
+    <t>TATA-SERVER-02</t>
+  </si>
+  <si>
+    <t>TATA_SERVER-03</t>
+  </si>
+  <si>
+    <t>TATA_SERVER-04</t>
+  </si>
+  <si>
+    <t>TATA_SERVER-05</t>
+  </si>
+  <si>
+    <t>TATA_SERVER-06</t>
+  </si>
+  <si>
+    <t>TATA_SERVER-07</t>
+  </si>
+  <si>
+    <t>TATA_SERVER-08</t>
+  </si>
+  <si>
+    <t>238.77.25.91</t>
+  </si>
+  <si>
+    <t>238.77.25.92</t>
+  </si>
+  <si>
+    <t>238.77.25.93</t>
+  </si>
+  <si>
+    <t>238.77.25.94</t>
+  </si>
+  <si>
+    <t>238.77.25.95</t>
+  </si>
+  <si>
+    <t>238.77.25.96</t>
+  </si>
+  <si>
+    <t>238.77.25.97</t>
+  </si>
+  <si>
+    <t>238.77.25.98</t>
+  </si>
+  <si>
+    <t>cinemax</t>
+  </si>
+  <si>
+    <t>10.77.22.5</t>
+  </si>
+  <si>
+    <t>239.77.16.5</t>
+  </si>
+  <si>
+    <t>A&amp;E HD</t>
+  </si>
+  <si>
+    <t>AMC HD</t>
+  </si>
+  <si>
+    <t>Cinemax Panamericano HD</t>
+  </si>
+  <si>
+    <t>Cinemax South HD</t>
+  </si>
+  <si>
+    <t>CNN International</t>
+  </si>
+  <si>
+    <t>El Gourmet HD</t>
+  </si>
+  <si>
+    <t>Golden TV</t>
+  </si>
+  <si>
+    <t>Hola TV HD</t>
+  </si>
+  <si>
+    <t>Lifetime HD</t>
+  </si>
+  <si>
+    <t>Nickelodeon HD</t>
+  </si>
+  <si>
+    <t>Paramount</t>
+  </si>
+  <si>
+    <t>Sony Entertainment</t>
+  </si>
+  <si>
+    <t>Space (Sur)</t>
+  </si>
+  <si>
+    <t>Space HD</t>
+  </si>
+  <si>
+    <t>TNT Series</t>
+  </si>
+  <si>
+    <t>Warner Channel</t>
+  </si>
+  <si>
+    <t>10.77.22.24</t>
+  </si>
+  <si>
+    <t>10.77.22.7</t>
+  </si>
+  <si>
+    <t>10.77.22.8</t>
+  </si>
+  <si>
+    <t>10.77.22.64</t>
+  </si>
+  <si>
+    <t>10.77.22.14</t>
+  </si>
+  <si>
+    <t>10.77.22.23</t>
+  </si>
+  <si>
+    <t>10.77.22.10</t>
+  </si>
+  <si>
+    <t>10.77.22.12</t>
+  </si>
+  <si>
+    <t>10.77.22.13</t>
+  </si>
+  <si>
+    <t>10.77.22.22</t>
+  </si>
+  <si>
+    <t>10.77.22.27</t>
+  </si>
+  <si>
+    <t>10.77.22.1</t>
+  </si>
+  <si>
+    <t>10.77.22.2</t>
+  </si>
+  <si>
+    <t>10.77.22.15</t>
+  </si>
+  <si>
+    <t>10.77.22.30</t>
+  </si>
+  <si>
+    <t>239.77.16.24</t>
+  </si>
+  <si>
+    <t>239.77.16.7</t>
+  </si>
+  <si>
+    <t>239.77.16.8</t>
+  </si>
+  <si>
+    <t>239.77.16.64</t>
+  </si>
+  <si>
+    <t>239.77.16.14</t>
+  </si>
+  <si>
+    <t>239.77.16.23</t>
+  </si>
+  <si>
+    <t>239.77.16.10</t>
+  </si>
+  <si>
+    <t>239.77.16.12</t>
+  </si>
+  <si>
+    <t>239.77.16.13</t>
+  </si>
+  <si>
+    <t>239.77.16.22</t>
+  </si>
+  <si>
+    <t>239.77.16.27</t>
+  </si>
+  <si>
+    <t>239.77.16.1</t>
+  </si>
+  <si>
+    <t>239.77.16.2</t>
+  </si>
+  <si>
+    <t>239.77.16.15</t>
+  </si>
+  <si>
+    <t>239.77.16.30</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>239.77.16.222</t>
+  </si>
+  <si>
+    <t>cisco server 8</t>
+  </si>
+  <si>
+    <t>10.77.22.222</t>
+  </si>
+  <si>
+    <t>Golden TV ird_out</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -508,7 +837,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -623,6 +952,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -668,9 +1045,23 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -691,11 +1082,10 @@
     <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
@@ -712,31 +1102,66 @@
     <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D6FF4EE4-C3D8-41C0-BE58-187ED69D9505}" name="Table1" displayName="Table1" ref="A1:B21" totalsRowShown="0">
-  <autoFilter ref="A1:B21" xr:uid="{D6FF4EE4-C3D8-41C0-BE58-187ED69D9505}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:F33" totalsRowShown="0">
+  <autoFilter ref="A1:F33"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="titulo"/>
+    <tableColumn id="2" name="protocolo"/>
+    <tableColumn id="3" name="fuente"/>
+    <tableColumn id="4" name="ip" dataDxfId="1"/>
+    <tableColumn id="5" name="puerto"/>
+    <tableColumn id="6" name="url"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B21" totalsRowShown="0">
+  <autoFilter ref="A1:B21"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{8251786E-ACE5-4D80-854D-B37E02C85238}" name="fuente"/>
-    <tableColumn id="2" xr3:uid="{9E81824E-1DFC-4FBC-9F59-C0A1E8C72331}" name="titulo"/>
+    <tableColumn id="1" name="fuente"/>
+    <tableColumn id="2" name="titulo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla24" displayName="Tabla24" ref="A1:F14" totalsRowShown="0">
+  <autoFilter ref="A1:F14"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="titulo"/>
+    <tableColumn id="2" name="protocolo"/>
+    <tableColumn id="3" name="fuente"/>
+    <tableColumn id="4" name="ip" dataDxfId="0"/>
+    <tableColumn id="5" name="puerto"/>
+    <tableColumn id="6" name="url"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
@@ -783,7 +1208,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -835,7 +1260,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1029,81 +1454,663 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{022B1446-91E5-403A-AE66-59E9B3592BA3}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2">
-        <v>12901</v>
+      <c r="F1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="7">
+        <v>10000</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="9">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="4">
+        <v>8999</v>
+      </c>
+      <c r="F10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="E11" s="15">
+        <v>8999</v>
+      </c>
+      <c r="F11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E12" s="4">
+        <v>8999</v>
+      </c>
+      <c r="F12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" s="4">
+        <v>8999</v>
+      </c>
+      <c r="F13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E14" s="4">
+        <v>8999</v>
+      </c>
+      <c r="F14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E15" s="4">
+        <v>8999</v>
+      </c>
+      <c r="F15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" s="4">
+        <v>8999</v>
+      </c>
+      <c r="F16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" s="4">
+        <v>8999</v>
+      </c>
+      <c r="F17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" s="4">
+        <v>8999</v>
+      </c>
+      <c r="F18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E19" s="4">
+        <v>8999</v>
+      </c>
+      <c r="F19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E20" s="4">
+        <v>8999</v>
+      </c>
+      <c r="F20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E21" s="4">
+        <v>8999</v>
+      </c>
+      <c r="F21" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E22" s="4">
+        <v>8999</v>
+      </c>
+      <c r="F22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E23" s="4">
+        <v>8999</v>
+      </c>
+      <c r="F23" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E24" s="4">
+        <v>8999</v>
+      </c>
+      <c r="F24" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25" s="11">
+        <v>8999</v>
+      </c>
+      <c r="F25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" t="s">
+        <v>135</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E33">
+        <v>8000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1116,7 +2123,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
@@ -1234,7 +2241,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1242,7 +2249,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1250,7 +2257,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1258,7 +2265,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1266,12 +2273,573 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="4">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="4">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="4">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="4">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="4">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="4">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="4">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E29" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E30" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E32" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E33" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E34" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E35" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E36" s="9">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E37" s="4">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E38" s="4">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E39" s="4">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E40" s="4">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" s="4">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E42" s="4">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E43" s="4">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E44" s="4">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E45" s="4">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E46" s="4">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E47" s="4">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E48" s="4">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E49" s="4">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E50" s="4">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E51" s="4">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E52" s="4">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E53" s="11">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="E54" s="11">
+        <v>8999</v>
       </c>
     </row>
   </sheetData>
@@ -1283,381 +2851,387 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02A1634C-4566-4F87-A3C1-C5172E0D1497}">
-  <dimension ref="A1:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A5" sqref="A5:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="2">
+        <v>8000</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="2">
+        <v>8000</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="2">
+        <v>8000</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="2">
+        <v>8000</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="2">
+        <v>8000</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="2">
+        <v>8000</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="2">
+        <v>8000</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2">
-        <v>12901</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3">
-        <v>12002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4">
-        <v>12003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5">
-        <v>12004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6">
-        <v>12005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7">
-        <v>12006</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8">
-        <v>12007</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9">
-        <v>12008</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10">
-        <v>12009</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11">
-        <v>12010</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12">
-        <v>12011</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13">
-        <v>12012</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14">
-        <v>12013</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15">
-        <v>12014</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16">
-        <v>12015</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17">
-        <v>12016</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18">
-        <v>12017</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="E19">
-        <v>12018</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>10090</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="E20">
-        <v>12019</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="E21">
-        <v>12020</v>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>